<commit_message>
added xlabel support to location.boxplot
</commit_message>
<xml_diff>
--- a/wqio/data/testtable_toXL.xlsx
+++ b/wqio/data/testtable_toXL.xlsx
@@ -399,75 +399,75 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:5">
-      <c r="A1" s="1" t="s">
+    <row spans="1:5" r="1">
+      <c s="1" t="s" r="A1">
         <v>4</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c s="1" t="s" r="B1">
         <v>0</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c s="1" t="s" r="C1">
         <v>1</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c s="1" t="s" r="D1">
         <v>2</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c s="1" t="s" r="E1">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:5">
-      <c r="A2" t="s">
+    <row spans="1:5" r="2">
+      <c t="s" r="A2">
         <v>5</v>
       </c>
-      <c r="B2" t="n">
+      <c t="n" r="B2">
         <v>1</v>
       </c>
-      <c r="C2" t="n">
+      <c t="n" r="C2">
         <v>2</v>
       </c>
-      <c r="D2" t="n">
+      <c t="n" r="D2">
         <v>3</v>
       </c>
-      <c r="E2" t="n">
+      <c t="n" r="E2">
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:5">
-      <c r="A3" t="s">
+    <row spans="1:5" r="3">
+      <c t="s" r="A3">
         <v>6</v>
       </c>
-      <c r="B3" t="n">
+      <c t="n" r="B3">
         <v>5</v>
       </c>
-      <c r="C3" t="n">
+      <c t="n" r="C3">
         <v>6</v>
       </c>
-      <c r="D3" t="n">
+      <c t="n" r="D3">
         <v>7</v>
       </c>
-      <c r="E3" t="n">
+      <c t="n" r="E3">
         <v>8</v>
       </c>
     </row>
-    <row r="4" spans="1:5">
-      <c r="A4" t="s">
+    <row spans="1:5" r="4">
+      <c t="s" r="A4">
         <v>7</v>
       </c>
-      <c r="B4" t="n">
+      <c t="n" r="B4">
         <v>9</v>
       </c>
-      <c r="C4" t="n">
+      <c t="n" r="C4">
         <v>0</v>
       </c>
-      <c r="D4" t="n">
+      <c t="n" r="D4">
         <v>1</v>
       </c>
-      <c r="E4" t="n">
+      <c t="n" r="E4">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" left="0.75" footer="0.5" top="1" bottom="1" header="0.5"/>
+  <pageMargins right="0.75" header="0.5" left="0.75" footer="0.5" top="1" bottom="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
categorical histogram support functions
_classifier takes a value and bins and returns e.g., "5 - 10" for
_classifier(7, [5, 10 ,15])
_unique_categories takes the same bins and compute all possible output
from _classifier
</commit_message>
<xml_diff>
--- a/wqio/data/testtable_toXL.xlsx
+++ b/wqio/data/testtable_toXL.xlsx
@@ -1,22 +1,24 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<s:workbook xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <s:workbookPr codeName="ThisWorkbook" defaultThemeVersion="124226"/>
+<s:workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:workbookPr/>
   <s:bookViews>
-    <s:workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
+    <s:workbookView activeTab="0"/>
   </s:bookViews>
   <s:sheets>
-    <s:sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" r:id="rId1"/>
+    <s:sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </s:sheets>
   <s:definedNames/>
-  <s:calcPr calcId="124519" calcMode="auto" fullCalcOnLoad="1"/>
+  <s:calcPr calcId="124519" fullCalcOnLoad="1"/>
 </s:workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="8">
   <si>
+    <t>Date</t>
+  </si>
+  <si>
     <t>A</t>
   </si>
   <si>
@@ -27,9 +29,6 @@
   </si>
   <si>
     <t>D</t>
-  </si>
-  <si>
-    <t>Date</t>
   </si>
   <si>
     <t>X</t>
@@ -48,23 +47,23 @@
   <numFmts count="0"/>
   <fonts count="2">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11.0"/>
-      <color rgb="00000000"/>
       <name val="Calibri"/>
       <family val="2"/>
-      <b/>
+      <b val="1"/>
+      <color rgb="00000000"/>
+      <sz val="11"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
@@ -89,9 +88,9 @@
   <cellStyleXfs count="1">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf borderId="0" fillId="0" fontId="0" numFmtId="0" xfId="0"/>
-    <xf applyAlignment="1" applyBorder="1" applyFont="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
+    <xf applyAlignment="1" borderId="1" fillId="0" fontId="1" numFmtId="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
@@ -387,87 +386,88 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr>
-    <outlinePr summaryBelow="1" summaryRight="1"/>
-  </sheetPr>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+    <s:outlinePr summaryBelow="1" summaryRight="1"/>
+    <s:pageSetUpPr/>
+  </s:sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1" activeCell="A1"/>
+      <selection activeCell="A1" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row spans="1:5" r="1">
-      <c s="1" t="s" r="A1">
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>4</v>
       </c>
-      <c s="1" t="s" r="B1">
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E2" t="n">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" t="n">
+        <v>6</v>
+      </c>
+      <c r="D3" t="n">
+        <v>7</v>
+      </c>
+      <c r="E3" t="n">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="n">
+        <v>9</v>
+      </c>
+      <c r="C4" t="n">
         <v>0</v>
       </c>
-      <c s="1" t="s" r="C1">
+      <c r="D4" t="n">
         <v>1</v>
       </c>
-      <c s="1" t="s" r="D1">
-        <v>2</v>
-      </c>
-      <c s="1" t="s" r="E1">
-        <v>3</v>
-      </c>
-    </row>
-    <row spans="1:5" r="2">
-      <c t="s" r="A2">
-        <v>5</v>
-      </c>
-      <c t="n" r="B2">
-        <v>1</v>
-      </c>
-      <c t="n" r="C2">
-        <v>2</v>
-      </c>
-      <c t="n" r="D2">
-        <v>3</v>
-      </c>
-      <c t="n" r="E2">
-        <v>4</v>
-      </c>
-    </row>
-    <row spans="1:5" r="3">
-      <c t="s" r="A3">
-        <v>6</v>
-      </c>
-      <c t="n" r="B3">
-        <v>5</v>
-      </c>
-      <c t="n" r="C3">
-        <v>6</v>
-      </c>
-      <c t="n" r="D3">
-        <v>7</v>
-      </c>
-      <c t="n" r="E3">
-        <v>8</v>
-      </c>
-    </row>
-    <row spans="1:5" r="4">
-      <c t="s" r="A4">
-        <v>7</v>
-      </c>
-      <c t="n" r="B4">
-        <v>9</v>
-      </c>
-      <c t="n" r="C4">
-        <v>0</v>
-      </c>
-      <c t="n" r="D4">
-        <v>1</v>
-      </c>
-      <c t="n" r="E4">
+      <c r="E4" t="n">
         <v>2</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins right="0.75" header="0.5" left="0.75" footer="0.5" top="1" bottom="1"/>
+  <pageMargins bottom="1" footer="0.5" header="0.5" left="0.75" right="0.75" top="1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
new test images for mpl1.5.1
</commit_message>
<xml_diff>
--- a/wqio/data/testtable_toXL.xlsx
+++ b/wqio/data/testtable_toXL.xlsx
@@ -95,7 +95,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle builtinId="0" name="Normal" xfId="0"/>
+    <cellStyle builtinId="0" hidden="0" name="Normal" xfId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultPivotStyle="PivotStyleLight16" defaultTableStyle="TableStyleMedium9"/>
@@ -387,10 +387,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <s:sheetPr xmlns:s="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-    <s:outlinePr summaryBelow="1" summaryRight="1"/>
-    <s:pageSetUpPr/>
-  </s:sheetPr>
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
   <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView workbookViewId="0">

</xml_diff>